<commit_message>
Testing Save Excel Function
</commit_message>
<xml_diff>
--- a/Images/Workbook_2.xlsx
+++ b/Images/Workbook_2.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$G$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$G$43</definedName>
   </definedNames>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>DATE</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Cashier Signature</t>
   </si>
   <si>
-    <t>Guest Signature</t>
-  </si>
-  <si>
     <t>Page 1-1</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Delivered</t>
   </si>
   <si>
-    <t>Paid</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -96,12 +90,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>oiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiii</t>
-  </si>
-  <si>
-    <t>GSTIN No:</t>
-  </si>
-  <si>
     <t xml:space="preserve">         Thanks for Choosing Wash &amp; Fold Laundry Services</t>
   </si>
   <si>
@@ -126,10 +114,31 @@
     <t>Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: You are not authorized to upload this format to any online  / offline medium without the permission of Spyderweb Technologies Inc.©   </t>
-  </si>
-  <si>
     <t>Bill Made Using:- Techware BillSoft.</t>
+  </si>
+  <si>
+    <t>SHIPPING</t>
+  </si>
+  <si>
+    <t>Payment Due:-</t>
+  </si>
+  <si>
+    <t>0$</t>
+  </si>
+  <si>
+    <t>©Spyderweb Technologies Inc.</t>
+  </si>
+  <si>
+    <t>Note: You are not authorized to upload this format to any online  / offline medium without the permission of Wash &amp; Fold Laundry©</t>
+  </si>
+  <si>
+    <t>Customer Signature</t>
+  </si>
+  <si>
+    <t>&lt;Employee Name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Address&gt;</t>
   </si>
 </sst>
 </file>
@@ -267,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -366,9 +375,44 @@
     </border>
     <border>
       <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="hair">
         <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.24994659260841701"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -377,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -438,9 +482,6 @@
     <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -448,77 +489,101 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,16 +606,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>449250</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>73725</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1173150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>988125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -567,7 +632,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="180975" y="4848225"/>
+          <a:off x="4248150" y="85725"/>
           <a:ext cx="2030400" cy="902400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -869,7 +934,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -879,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:D15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -892,84 +957,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="84.95" customHeight="1">
-      <c r="A1" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="A1" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
+        <v>17</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="20">
+        <v>1</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="23">
-        <v>1</v>
-      </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="5" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -978,452 +1041,439 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="E8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="19" t="s">
-        <v>15</v>
+      <c r="A9" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="39">
+      <c r="E9" s="31">
         <v>43194</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="19" t="s">
-        <v>20</v>
+      <c r="A10" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
+      <c r="E10" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="19" t="s">
-        <v>19</v>
+      <c r="A11" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="39">
+      <c r="E11" s="31">
         <v>43194</v>
       </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A12" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="38" t="s">
+      <c r="A12" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="20" t="s">
+      <c r="A16" s="28" t="s">
         <v>21</v>
       </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="9">
-        <f>IF(E17="",ROUND(1*F17,2),ROUND(E17*F17,2))</f>
-        <v>0</v>
-      </c>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="12">
-        <f>IF(E18="",ROUND(1*F18,2),ROUND(E18*F18,2))</f>
-        <v>0</v>
-      </c>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="12">
-        <f>IF(E19="",ROUND(1*F19,2),ROUND(E19*F19,2))</f>
-        <v>0</v>
-      </c>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="11"/>
-      <c r="G20" s="12">
-        <f>IF(E20="",ROUND(1*F20,2),ROUND(E20*F20,2))</f>
-        <v>0</v>
-      </c>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="12">
-        <f t="shared" ref="G21:G26" si="0">IF(E21="",ROUND(1*F21,2),ROUND(E21*F21,2))</f>
-        <v>0</v>
-      </c>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="42"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
-      <c r="G24" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="11"/>
-      <c r="G25" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="42"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="42"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="11"/>
-      <c r="G27" s="12">
-        <f>IF(E27="",ROUND(1*F27,2),ROUND(E27*F27,2))</f>
-        <v>0</v>
-      </c>
+      <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="42"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="11"/>
-      <c r="G28" s="12">
-        <f>IF(E28="",ROUND(1*F28,2),ROUND(E28*F28,2))</f>
-        <v>0</v>
-      </c>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="42"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
-      <c r="G29" s="12">
-        <f>IF(E29="",ROUND(1*F29,2),ROUND(E29*F29,2))</f>
-        <v>0</v>
-      </c>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="12">
-        <f>IF(E30="",ROUND(1*F30,2),ROUND(E30*F30,2))</f>
-        <v>0</v>
-      </c>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="42"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="16">
-        <f>IF(E31="",ROUND(1*F31,2),ROUND(E31*F31,2))</f>
-        <v>0</v>
-      </c>
+      <c r="G31" s="16"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="21" t="s">
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="21"/>
-      <c r="G32" s="17">
-        <f>SUM(G17:G31)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="18.75">
-      <c r="A33" s="35"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="21" t="s">
+      <c r="F32" s="44"/>
+      <c r="G32" s="17"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="43"/>
+      <c r="G33" s="47"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="43"/>
+      <c r="G34" s="47"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="45"/>
+      <c r="G35" s="48"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="1:7" ht="18.75">
-      <c r="A34" s="35"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F34" s="22"/>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A35" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="33" t="s">
+      <c r="G40" s="29"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A41" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37" t="s">
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="29"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A42" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="G39" s="37"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A41" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+    </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B2:D4"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A12:D15"/>
+  <mergeCells count="43">
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A41:G42"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A32:D34"/>
+    <mergeCell ref="A42:G43"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="A38:C38"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G36"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E9:G9"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B2:D4"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A12:D15"/>
+    <mergeCell ref="A32:D35"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="F39:G39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>